<commit_message>
Starting the ending of a raid.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/raids.xlsx
+++ b/resources/data-imports/Admin Section/raids.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>name</t>
   </si>
@@ -35,6 +35,9 @@
     <t>corrupted_location_ids</t>
   </si>
   <si>
+    <t>item_specialty_reward_type</t>
+  </si>
+  <si>
     <t>The Smugglers Are Back!</t>
   </si>
   <si>
@@ -51,6 +54,9 @@
   </si>
   <si>
     <t>Smugglers Port,Dalix,Port of Salix,Karth</t>
+  </si>
+  <si>
+    <t>Pirate Lord Leather</t>
   </si>
 </sst>
 </file>
@@ -390,7 +396,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -404,9 +410,10 @@
     <col min="4" max="4" width="150.963" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="25.851" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="48.274" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="31.707" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,25 +432,31 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started working on the Affix Generator.
- The exponential curve generator for levels and other required stats is finally in place.
- Other minor changes and fixes.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/raids.xlsx
+++ b/resources/data-imports/Admin Section/raids.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>name</t>
   </si>
@@ -38,6 +38,9 @@
     <t>item_specialty_reward_type</t>
   </si>
   <si>
+    <t>artifact_item_id</t>
+  </si>
+  <si>
     <t>The Smugglers Are Back!</t>
   </si>
   <si>
@@ -57,6 +60,9 @@
   </si>
   <si>
     <t>Pirate Lord Leather</t>
+  </si>
+  <si>
+    <t>Ancestral Finger Bone of The Magi Troth</t>
   </si>
 </sst>
 </file>
@@ -396,7 +402,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -411,9 +417,10 @@
     <col min="5" max="5" width="25.851" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="48.274" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="31.707" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="47.131" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,28 +442,34 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>